<commit_message>
Added some more jobs
</commit_message>
<xml_diff>
--- a/sankyDiagram/applicationProcessData.xlsx
+++ b/sankyDiagram/applicationProcessData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/412ae8e0f3501a03/Skrivskit/LETA JOBB/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/412ae8e0f3501a03/Skrivskit/LETA JOBB/Sankey-diagram-for-job-search/sankyDiagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="11_AD4D7A0C205A6B9A452FA8663FD5D944693EDF14" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{95BC0D10-6F0A-43A2-8EB1-480C1D6DA293}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="11_AD4D7A0C205A6B9A452FA8663FD5D944693EDF14" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{56BCD21D-E66A-4C81-BABB-2B0EA119E341}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
   <si>
     <t>TYPE</t>
   </si>
@@ -54,9 +54,6 @@
     <t>SCANIA Young Potential Trainee program</t>
   </si>
   <si>
-    <t>Replies</t>
-  </si>
-  <si>
     <t>Logic and personality test</t>
   </si>
   <si>
@@ -79,6 +76,33 @@
   </si>
   <si>
     <t>SOLITA Data academy</t>
+  </si>
+  <si>
+    <t>ERICSSON Next Generation Talent</t>
+  </si>
+  <si>
+    <t>SEB Junior Data engineer</t>
+  </si>
+  <si>
+    <t>ATEA Intelligent Automation och RPA-konsult</t>
+  </si>
+  <si>
+    <t>Arbetsförmedlingen</t>
+  </si>
+  <si>
+    <t>Replied</t>
+  </si>
+  <si>
+    <t>Interview 1</t>
+  </si>
+  <si>
+    <t>TietoEVRY</t>
+  </si>
+  <si>
+    <t>Reference check</t>
+  </si>
+  <si>
+    <t>SCANIA Developer engineer 2</t>
   </si>
 </sst>
 </file>
@@ -406,20 +430,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="38.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -442,7 +467,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -459,13 +484,13 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" t="s">
         <v>9</v>
       </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -473,7 +498,7 @@
         <v>44271</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -482,7 +507,10 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -490,7 +518,7 @@
         <v>44282</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
         <v>1</v>
@@ -499,7 +527,13 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="F4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -507,16 +541,110 @@
         <v>44283</v>
       </c>
       <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>44285</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E5" t="s">
-        <v>14</v>
+      <c r="C6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>44285</v>
+      </c>
+      <c r="B7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>44289</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>44290</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>44299</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added better link and node colors, writes out node counts
</commit_message>
<xml_diff>
--- a/sankyDiagram/applicationProcessData.xlsx
+++ b/sankyDiagram/applicationProcessData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/412ae8e0f3501a03/Skrivskit/LETA JOBB/Sankey-diagram-for-job-search/sankyDiagram/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="100" documentId="11_AD4D7A0C205A6B9A452FA8663FD5D944693EDF14" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{56BCD21D-E66A-4C81-BABB-2B0EA119E341}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="11_AD4D7A0C205A6B9A452FA8663FD5D944693EDF14" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1DDF424F-444A-4503-8C62-98F03E402806}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="34">
   <si>
     <t>TYPE</t>
   </si>
@@ -66,9 +66,6 @@
     <t>FOI Biträdande analytiker</t>
   </si>
   <si>
-    <t>Waiting for reply</t>
-  </si>
-  <si>
     <t>SCANIA Developer engineer</t>
   </si>
   <si>
@@ -103,13 +100,40 @@
   </si>
   <si>
     <t>SCANIA Developer engineer 2</t>
+  </si>
+  <si>
+    <t>No reply</t>
+  </si>
+  <si>
+    <t>Invited to video interview</t>
+  </si>
+  <si>
+    <t>RESULT_4</t>
+  </si>
+  <si>
+    <t>Declined</t>
+  </si>
+  <si>
+    <t>Code test</t>
+  </si>
+  <si>
+    <t>RESULT_5</t>
+  </si>
+  <si>
+    <t>Offer</t>
+  </si>
+  <si>
+    <t>RESULT_6</t>
+  </si>
+  <si>
+    <t>Accepted</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,6 +145,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -430,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -444,10 +474,10 @@
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="24.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -469,13 +499,22 @@
       <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>44269</v>
+        <v>44285</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
         <v>1</v>
@@ -484,84 +523,105 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>44290</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>44283</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>44271</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>44282</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>7</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E5" t="s">
+        <v>20</v>
+      </c>
+      <c r="F5" t="s">
         <v>21</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>44282</v>
-      </c>
-      <c r="B4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>44283</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
-        <v>44285</v>
+        <v>44269</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C6" t="s">
         <v>1</v>
@@ -570,72 +630,75 @@
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F6" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
+        <v>44271</v>
+      </c>
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>44285</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>44289</v>
+      </c>
+      <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>44289</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>44290</v>
-      </c>
-      <c r="B9" t="s">
-        <v>23</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>15</v>
-      </c>
       <c r="E9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44299</v>
       </c>
       <c r="B10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
         <v>1</v>
@@ -644,10 +707,18 @@
         <v>7</v>
       </c>
       <c r="E10" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J9">
+    <sortCondition ref="J2:J9"/>
+    <sortCondition ref="I2:I9"/>
+    <sortCondition ref="H2:H9"/>
+    <sortCondition ref="G2:G9"/>
+    <sortCondition ref="F2:F9"/>
+  </sortState>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>